<commit_message>
Add export button and change the page title
</commit_message>
<xml_diff>
--- a/bug_report.xlsx
+++ b/bug_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -710,6 +710,37 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>hhh not seen</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>fixed</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+            Passed</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2023-07-28 11:04:09</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2023-07-28 11:04:28</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
css table seperated and updated the button colors and change the bug report table position
</commit_message>
<xml_diff>
--- a/bug_report.xlsx
+++ b/bug_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -741,6 +741,85 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ffg not working</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2023-07-28 12:38:00</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>io none</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>io none</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2023-07-28 12:41:13</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>er fgv</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>er fgv fixed</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+            Passed</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2023-07-28 16:13:23</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2023-07-28 16:15:07</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>